<commit_message>
Updated images, updated evaluation section with descriptions, new images, distance table, changed image sizes, added some background details.
</commit_message>
<xml_diff>
--- a/report/Benchmark_concurrent_connections.xlsx
+++ b/report/Benchmark_concurrent_connections.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gebruiker\Documents\GM-Web-Multiplayer\report\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="60" windowWidth="24915" windowHeight="12840"/>
   </bookViews>
@@ -70,13 +75,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -85,7 +93,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -103,10 +111,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.18650874707607157"/>
+          <c:x val="0.12385415053686094"/>
           <c:y val="6.2708151064450282E-2"/>
-          <c:w val="0.79088261456857634"/>
-          <c:h val="0.61388086905803441"/>
+          <c:w val="0.85353719975485609"/>
+          <c:h val="0.67406605424321964"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -126,6 +134,17 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:tint val="88500"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -613,14 +632,26 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:hiLowLines/>
-        <c:marker val="1"/>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="45068288"/>
-        <c:axId val="45069824"/>
+        <c:axId val="80980784"/>
+        <c:axId val="80986768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="45068288"/>
+        <c:axId val="80980784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -629,11 +660,21 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400"/>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB" sz="1400"/>
@@ -644,22 +685,72 @@
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400"/>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45069824"/>
+        <c:crossAx val="80986768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -667,21 +758,44 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="45069824"/>
+        <c:axId val="80986768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400"/>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB" sz="1400"/>
@@ -692,54 +806,106 @@
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400"/>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45068288"/>
+        <c:crossAx val="80980784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.20015308755861588"/>
-          <c:y val="7.8511592300962385E-2"/>
-          <c:w val="0.20814349342584978"/>
-          <c:h val="9.4923811606882458E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -751,7 +917,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -769,10 +935,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.19842616749097944"/>
+          <c:x val="0.12247077939656291"/>
           <c:y val="6.8356663750364532E-2"/>
-          <c:w val="0.76763284382573149"/>
-          <c:h val="0.6195286526684165"/>
+          <c:w val="0.84358808738669655"/>
+          <c:h val="0.68897309711286081"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -792,6 +958,17 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:tint val="88500"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1279,14 +1456,26 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:hiLowLines/>
-        <c:marker val="1"/>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="47016576"/>
-        <c:axId val="47114112"/>
+        <c:axId val="80992208"/>
+        <c:axId val="80981328"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="47016576"/>
+        <c:axId val="80992208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1295,11 +1484,21 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400"/>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB" sz="1400"/>
@@ -1310,22 +1509,72 @@
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400"/>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47114112"/>
+        <c:crossAx val="80981328"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1333,21 +1582,44 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47114112"/>
+        <c:axId val="80981328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400"/>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB" sz="1400"/>
@@ -1358,54 +1630,106 @@
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400"/>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47016576"/>
+        <c:crossAx val="80992208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.21397747369489012"/>
-          <c:y val="8.0768810148731413E-2"/>
-          <c:w val="0.27766710411198603"/>
-          <c:h val="9.4923811606882458E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -1417,7 +1741,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="nl-NL"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1435,10 +1759,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.22446182250407601"/>
+          <c:x val="0.15038986731191356"/>
           <c:y val="6.2592592592592602E-2"/>
-          <c:w val="0.74612749665448241"/>
-          <c:h val="0.61399642752989214"/>
+          <c:w val="0.82019948532628184"/>
+          <c:h val="0.67881124234470691"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1458,6 +1782,17 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="dk1">
+                  <a:tint val="88500"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
@@ -1945,14 +2280,26 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:hiLowLines/>
-        <c:marker val="1"/>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="57768192"/>
-        <c:axId val="57786368"/>
+        <c:axId val="80990032"/>
+        <c:axId val="80983504"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57768192"/>
+        <c:axId val="80990032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1961,11 +2308,21 @@
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400"/>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB" sz="1400"/>
@@ -1976,22 +2333,72 @@
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400"/>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57786368"/>
+        <c:crossAx val="80983504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1999,24 +2406,47 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57786368"/>
+        <c:axId val="80983504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
-              <a:bodyPr/>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1400"/>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB" sz="1400"/>
+                  <a:rPr lang="en-GB" sz="1400" b="0"/>
                   <a:t>CPU Time (ms)</a:t>
                 </a:r>
               </a:p>
@@ -2024,60 +2454,1741 @@
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="nl-NL"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
         <c:txPr>
-          <a:bodyPr/>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400"/>
+              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="nl-NL"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57768192"/>
+        <c:crossAx val="80990032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.22916498897267978"/>
-          <c:y val="5.7620662000583252E-2"/>
-          <c:w val="0.27715522113673385"/>
-          <c:h val="9.4923811606882458E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="nl-NL"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="20">
+  <a:schemeClr val="dk1"/>
+  <cs:variation>
+    <a:tint val="88500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="55000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="75000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="98500"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:tint val="80000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2090,8 +4201,8 @@
       <xdr:rowOff>147371</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>345503</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>292234</xdr:colOff>
       <xdr:row>76</xdr:row>
       <xdr:rowOff>33071</xdr:rowOff>
     </xdr:to>
@@ -2115,13 +4226,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>78441</xdr:colOff>
+      <xdr:colOff>78440</xdr:colOff>
       <xdr:row>46</xdr:row>
       <xdr:rowOff>68355</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>414618</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>60</xdr:row>
       <xdr:rowOff>144555</xdr:rowOff>
     </xdr:to>
@@ -2145,13 +4256,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>81643</xdr:colOff>
+      <xdr:colOff>81642</xdr:colOff>
       <xdr:row>30</xdr:row>
       <xdr:rowOff>183324</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>410688</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>374291</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>69024</xdr:rowOff>
     </xdr:to>
@@ -2176,9 +4287,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Kantoor">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2216,9 +4327,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Kantoor">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2253,7 +4364,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2288,7 +4399,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Kantoor">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2464,8 +4575,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:G81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V66" sqref="V66"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="W44" sqref="W44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>